<commit_message>
Correct Test Case 1
</commit_message>
<xml_diff>
--- a/docs/Test Case 1.xlsx
+++ b/docs/Test Case 1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\OneDrive\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\maze-project-2021\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0C3A16F1-4A89-493D-B4CE-2AC80FF0E44A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9837882-5725-4F3A-A495-17B2C2214696}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5550" yWindow="4560" windowWidth="20235" windowHeight="11505" xr2:uid="{D88C0871-9CFF-47EC-A37B-1CA9AB3CB744}"/>
+    <workbookView xWindow="6735" yWindow="3390" windowWidth="20235" windowHeight="11505" xr2:uid="{D88C0871-9CFF-47EC-A37B-1CA9AB3CB744}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -123,15 +123,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thick">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thick">
         <color indexed="64"/>
       </left>
@@ -144,17 +135,6 @@
       <bottom style="thick">
         <color indexed="64"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thick">
-        <color indexed="64"/>
-      </left>
-      <right style="thick">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -198,15 +178,6 @@
         <color indexed="64"/>
       </right>
       <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thick">
-        <color indexed="64"/>
-      </right>
-      <top/>
       <bottom style="thick">
         <color indexed="64"/>
       </bottom>
@@ -219,6 +190,35 @@
       <right style="thick">
         <color indexed="64"/>
       </right>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right/>
       <top style="thick">
         <color indexed="64"/>
       </top>
@@ -231,53 +231,53 @@
   </cellStyleXfs>
   <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Нормален" xfId="0" builtinId="0"/>
@@ -597,7 +597,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1FB6EA0-B56F-4EA9-B144-2472D1E82256}">
-  <dimension ref="A1:J13"/>
+  <dimension ref="A1:J14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G1" sqref="G1"/>
@@ -615,136 +615,183 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="22.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="21" t="s">
+      <c r="C1" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="21" t="s">
+      <c r="D1" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="21" t="s">
+      <c r="E1" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="21" t="s">
+      <c r="F1" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="21" t="s">
+      <c r="G1" s="12" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="33" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="11">
+      <c r="A2" s="15">
         <v>1</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="D2" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="12" t="s">
+      <c r="E2" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="7"/>
-      <c r="G2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="2"/>
     </row>
     <row r="3" spans="1:10" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="16"/>
-      <c r="B3" s="17"/>
-      <c r="C3" s="14" t="s">
+      <c r="B3" s="14"/>
+      <c r="C3" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="15" t="s">
+      <c r="D3" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="13"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="6"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="3"/>
     </row>
     <row r="4" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2"/>
-      <c r="B4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="5"/>
-      <c r="I4" s="18"/>
-      <c r="J4" s="18"/>
+      <c r="A4" s="20"/>
+      <c r="B4" s="21"/>
+      <c r="C4" s="21"/>
+      <c r="D4" s="21"/>
+      <c r="E4" s="21"/>
+      <c r="F4" s="21"/>
+      <c r="G4" s="21"/>
+      <c r="H4" s="9"/>
+      <c r="I4" s="9"/>
+      <c r="J4" s="9"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="5"/>
+      <c r="A5" s="19"/>
+      <c r="B5" s="9"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
+      <c r="G5" s="9"/>
+      <c r="H5" s="9"/>
+      <c r="I5" s="9"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="5"/>
+      <c r="A6" s="19"/>
+      <c r="B6" s="9"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="9"/>
+      <c r="H6" s="9"/>
+      <c r="I6" s="9"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="2"/>
-      <c r="B7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="5"/>
+      <c r="A7" s="19"/>
+      <c r="B7" s="9"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="9"/>
+      <c r="H7" s="9"/>
+      <c r="I7" s="9"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="2"/>
-      <c r="B8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="5"/>
+      <c r="A8" s="19"/>
+      <c r="B8" s="9"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="9"/>
+      <c r="G8" s="9"/>
+      <c r="H8" s="9"/>
+      <c r="I8" s="9"/>
+      <c r="J8" s="9"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="2"/>
-      <c r="B9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="5"/>
+      <c r="A9" s="9"/>
+      <c r="B9" s="9"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="9"/>
+      <c r="H9" s="9"/>
+      <c r="I9" s="9"/>
+      <c r="J9" s="9"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="2"/>
-      <c r="B10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="5"/>
+      <c r="A10" s="9"/>
+      <c r="B10" s="9"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="9"/>
+      <c r="H10" s="9"/>
+      <c r="I10" s="9"/>
+      <c r="J10" s="9"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="2"/>
-      <c r="B11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="5"/>
-    </row>
-    <row r="12" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="3"/>
-      <c r="B12" s="3"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="6"/>
-    </row>
-    <row r="13" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+      <c r="A11" s="9"/>
+      <c r="B11" s="9"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="9"/>
+      <c r="G11" s="9"/>
+      <c r="H11" s="9"/>
+      <c r="I11" s="9"/>
+      <c r="J11" s="9"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="9"/>
+      <c r="B12" s="9"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="9"/>
+      <c r="F12" s="9"/>
+      <c r="G12" s="9"/>
+      <c r="H12" s="9"/>
+      <c r="I12" s="9"/>
+      <c r="J12" s="9"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="9"/>
+      <c r="B13" s="9"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="9"/>
+      <c r="F13" s="9"/>
+      <c r="G13" s="9"/>
+      <c r="H13" s="9"/>
+      <c r="I13" s="9"/>
+      <c r="J13" s="9"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="9"/>
+      <c r="B14" s="9"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="9"/>
+    </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="B2:B3"/>

</xml_diff>